<commit_message>
Added results for http and coap
</commit_message>
<xml_diff>
--- a/Results File.xlsx
+++ b/Results File.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\absonnie\CSC591-IOT-HW2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew\Documents\School\CSC591-IOT\CSC591-IOT-HW2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87C32C86-2F3B-4918-8F81-6C484159B694}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83F11D51-2E69-4752-A4A8-448BA6F81B1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4260" yWindow="1950" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -883,7 +883,7 @@
   <dimension ref="A1:Q7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1025,58 +1025,82 @@
       <c r="A6" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="5"/>
+      <c r="B6" s="4">
+        <v>597.81113861708502</v>
+      </c>
+      <c r="C6" s="2">
+        <v>2029.4212925735801</v>
+      </c>
+      <c r="D6" s="2">
+        <v>6318.0061176205299</v>
+      </c>
+      <c r="E6" s="2">
+        <v>26075.643014648202</v>
+      </c>
+      <c r="F6" s="2">
+        <v>5772.0237275871305</v>
+      </c>
+      <c r="G6" s="2">
+        <v>158178.70910074501</v>
+      </c>
+      <c r="H6" s="2">
+        <v>3513.3936214032301</v>
+      </c>
+      <c r="I6" s="5">
+        <v>10509.4771512315</v>
+      </c>
+      <c r="J6" s="14">
+        <v>0.38400000000000001</v>
+      </c>
+      <c r="K6" s="14">
+        <v>0.38400000000000001</v>
+      </c>
+      <c r="L6" s="14">
+        <v>0.38400000000000001</v>
+      </c>
+      <c r="M6" s="14">
+        <v>0.38400000000000001</v>
+      </c>
     </row>
     <row r="7" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
         <v>3</v>
       </c>
       <c r="B7" s="6">
-        <v>66.987611599896098</v>
+        <v>328.84254832621701</v>
       </c>
       <c r="C7" s="7">
-        <v>271.43564274302298</v>
+        <v>743.64511756416596</v>
       </c>
       <c r="D7" s="7">
-        <v>5395.7622633376204</v>
+        <v>35722.251096703898</v>
       </c>
       <c r="E7" s="7">
-        <v>37254.520513340402</v>
+        <v>1038535.99451121</v>
       </c>
       <c r="F7" s="7">
-        <v>524316.75549705897</v>
+        <v>1876659.7296289001</v>
       </c>
       <c r="G7" s="7">
-        <v>9393363.2527175099</v>
+        <v>45562676.805269897</v>
       </c>
       <c r="H7" s="7">
-        <v>4229125.5626010597</v>
+        <v>3489190.86420677</v>
       </c>
       <c r="I7" s="8">
-        <v>8216611.9865669403</v>
+        <v>21641500.804111298</v>
       </c>
       <c r="J7" s="15">
-        <v>1.17608</v>
+        <v>0.8</v>
       </c>
       <c r="K7" s="7">
-        <v>1.2579199999999999</v>
+        <v>81.92</v>
       </c>
       <c r="L7" s="7">
-        <v>85.054079999999999</v>
+        <v>8388.6080000000002</v>
       </c>
       <c r="M7" s="8">
-        <v>8257.3055999999997</v>
+        <v>82561.296000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed from qos 2 to qos 1 and excel sheet updated
</commit_message>
<xml_diff>
--- a/Results File.xlsx
+++ b/Results File.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10111"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew\Documents\School\CSC591-IOT\CSC591-IOT-HW2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arnabdatta/Desktop/CSC591-IOT-HW2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83F11D51-2E69-4752-A4A8-448BA6F81B1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA224CA3-FEE1-9649-B74F-6EE986D39E63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -883,17 +883,25 @@
   <dimension ref="A1:Q7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="13" width="10" customWidth="1"/>
-    <col min="14" max="17" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" customWidth="1"/>
+    <col min="3" max="3" width="14.1640625" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" customWidth="1"/>
+    <col min="5" max="5" width="14" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" customWidth="1"/>
+    <col min="7" max="7" width="14.5" customWidth="1"/>
+    <col min="8" max="8" width="21.1640625" customWidth="1"/>
+    <col min="9" max="9" width="22.33203125" customWidth="1"/>
+    <col min="10" max="13" width="10" customWidth="1"/>
+    <col min="14" max="17" width="9.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" s="34" t="s">
         <v>10</v>
       </c>
@@ -915,7 +923,7 @@
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B2" s="31" t="s">
         <v>5</v>
       </c>
@@ -949,7 +957,7 @@
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
     </row>
-    <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="22" t="s">
         <v>4</v>
       </c>
@@ -987,41 +995,73 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="10"/>
+      <c r="B4" s="3">
+        <v>83539.399999999994</v>
+      </c>
+      <c r="C4" s="9">
+        <v>17885.09</v>
+      </c>
+      <c r="D4" s="9">
+        <v>828635.17299999995</v>
+      </c>
+      <c r="E4" s="9">
+        <v>141518.14199999999</v>
+      </c>
+      <c r="F4" s="9">
+        <v>844990176.227</v>
+      </c>
+      <c r="G4" s="9">
+        <v>170006467.08500001</v>
+      </c>
+      <c r="H4" s="9">
+        <v>7041138301.8100004</v>
+      </c>
+      <c r="I4" s="10">
+        <v>3214330801.8800001</v>
+      </c>
       <c r="J4" s="16"/>
       <c r="K4" s="17"/>
       <c r="L4" s="17"/>
       <c r="M4" s="18"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="5"/>
+      <c r="B5" s="4">
+        <v>1668.6681000000001</v>
+      </c>
+      <c r="C5" s="2">
+        <v>682.29</v>
+      </c>
+      <c r="D5" s="2">
+        <v>17726.009999999998</v>
+      </c>
+      <c r="E5" s="2">
+        <v>7938.2</v>
+      </c>
+      <c r="F5" s="2">
+        <v>46784083.530000001</v>
+      </c>
+      <c r="G5" s="2">
+        <v>16843543.767000001</v>
+      </c>
+      <c r="H5" s="2">
+        <v>511400284.29500002</v>
+      </c>
+      <c r="I5" s="5">
+        <v>222389616.449</v>
+      </c>
       <c r="J5" s="14"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
       <c r="M5" s="5"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>2</v>
       </c>
@@ -1062,7 +1102,7 @@
         <v>0.38400000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
Mqtt qos2 2 (#4)
* mqtt-qos1 files

* removed output file

* one publish file created, dockerfiles modified

* dockerfile modified

* added mosquitto.conf

* testing qos 2

* Fixed docker

* Minor changes

* file transfer working

* changed from qos 2 to qos 1 and excel sheet updated

* fixed dockerfile

* changed qos input

Co-authored-by: adatta4 <adatta4@ncsu.edu>
Co-authored-by: arnab-95 <44353511+arnab-95@users.noreply.github.com>
Co-authored-by: alex-carruth <43625082+alex-carruth@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Results File.xlsx
+++ b/Results File.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10111"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew\Documents\School\CSC591-IOT\CSC591-IOT-HW2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arnabdatta/Desktop/CSC591-IOT-HW2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B7B7741-5D56-4F6C-9319-A20205FF65B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA224CA3-FEE1-9649-B74F-6EE986D39E63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -883,17 +883,25 @@
   <dimension ref="A1:Q7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="13" width="10" customWidth="1"/>
-    <col min="14" max="17" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" customWidth="1"/>
+    <col min="3" max="3" width="14.1640625" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" customWidth="1"/>
+    <col min="5" max="5" width="14" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" customWidth="1"/>
+    <col min="7" max="7" width="14.5" customWidth="1"/>
+    <col min="8" max="8" width="21.1640625" customWidth="1"/>
+    <col min="9" max="9" width="22.33203125" customWidth="1"/>
+    <col min="10" max="13" width="10" customWidth="1"/>
+    <col min="14" max="17" width="9.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" s="34" t="s">
         <v>10</v>
       </c>
@@ -915,7 +923,7 @@
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B2" s="31" t="s">
         <v>5</v>
       </c>
@@ -949,7 +957,7 @@
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
     </row>
-    <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="22" t="s">
         <v>4</v>
       </c>
@@ -987,41 +995,73 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="10"/>
+      <c r="B4" s="3">
+        <v>83539.399999999994</v>
+      </c>
+      <c r="C4" s="9">
+        <v>17885.09</v>
+      </c>
+      <c r="D4" s="9">
+        <v>828635.17299999995</v>
+      </c>
+      <c r="E4" s="9">
+        <v>141518.14199999999</v>
+      </c>
+      <c r="F4" s="9">
+        <v>844990176.227</v>
+      </c>
+      <c r="G4" s="9">
+        <v>170006467.08500001</v>
+      </c>
+      <c r="H4" s="9">
+        <v>7041138301.8100004</v>
+      </c>
+      <c r="I4" s="10">
+        <v>3214330801.8800001</v>
+      </c>
       <c r="J4" s="16"/>
       <c r="K4" s="17"/>
       <c r="L4" s="17"/>
       <c r="M4" s="18"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="5"/>
+      <c r="B5" s="4">
+        <v>1668.6681000000001</v>
+      </c>
+      <c r="C5" s="2">
+        <v>682.29</v>
+      </c>
+      <c r="D5" s="2">
+        <v>17726.009999999998</v>
+      </c>
+      <c r="E5" s="2">
+        <v>7938.2</v>
+      </c>
+      <c r="F5" s="2">
+        <v>46784083.530000001</v>
+      </c>
+      <c r="G5" s="2">
+        <v>16843543.767000001</v>
+      </c>
+      <c r="H5" s="2">
+        <v>511400284.29500002</v>
+      </c>
+      <c r="I5" s="5">
+        <v>222389616.449</v>
+      </c>
       <c r="J5" s="14"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
       <c r="M5" s="5"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>2</v>
       </c>
@@ -1062,7 +1102,7 @@
         <v>0.38400000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>3</v>
       </c>
@@ -1091,16 +1131,16 @@
         <v>21641500.804111298</v>
       </c>
       <c r="J7" s="15">
-        <v>1.1839999999999999</v>
+        <v>0.8</v>
       </c>
       <c r="K7" s="7">
-        <v>82.304000000000002</v>
+        <v>81.92</v>
       </c>
       <c r="L7" s="7">
-        <v>8388.9920000000002</v>
+        <v>8388.6080000000002</v>
       </c>
       <c r="M7" s="8">
-        <v>82561.679999999993</v>
+        <v>82561.296000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>